<commit_message>
First approaching to read xlsx file with daily patient information, now is reading an xlsx file and writing some information in the data base
</commit_message>
<xml_diff>
--- a/proofReading.xlsx
+++ b/proofReading.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>firstName</t>
   </si>
@@ -63,6 +63,24 @@
   </si>
   <si>
     <t>fx45544554</t>
+  </si>
+  <si>
+    <t>Sheldon</t>
+  </si>
+  <si>
+    <t>Cooper</t>
+  </si>
+  <si>
+    <t>03/23/1995</t>
+  </si>
+  <si>
+    <t>sheldon@bbt.com</t>
+  </si>
+  <si>
+    <t>otra dir 324</t>
+  </si>
+  <si>
+    <t>fx45544555</t>
   </si>
 </sst>
 </file>
@@ -107,9 +125,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -391,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,10 +464,38 @@
         <v>12</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>3434343434</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4" s="2"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" copies="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>